<commit_message>
code and style refresh and optimize
</commit_message>
<xml_diff>
--- a/htdocs/openaudit/out/testipscan.xlsx
+++ b/htdocs/openaudit/out/testipscan.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
-    <t>ÿþStatus</t>
+    <t>﻿Status</t>
   </si>
   <si>
     <t>Name</t>
@@ -133,7 +133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P4"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>

</xml_diff>